<commit_message>
add hbase node to i2up
</commit_message>
<xml_diff>
--- a/i2up/excel/template.xlsx
+++ b/i2up/excel/template.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sun_xo/learn/py/i2up/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E330BD-CCF0-014D-8E0A-BB1C96F71905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B1A8AB-D6AD-3448-AD15-6C3E1719A026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15180" activeTab="3" xr2:uid="{5EDD2148-16E0-F244-A20D-E769F585BB6C}"/>
+    <workbookView xWindow="-28240" yWindow="660" windowWidth="28040" windowHeight="15180" activeTab="1" xr2:uid="{5EDD2148-16E0-F244-A20D-E769F585BB6C}"/>
   </bookViews>
   <sheets>
     <sheet name="msq_node" sheetId="2" r:id="rId1"/>
-    <sheet name="kfk_node" sheetId="3" r:id="rId2"/>
-    <sheet name="msq_msq_rule" sheetId="4" r:id="rId3"/>
-    <sheet name="msq_kfk_rule" sheetId="5" r:id="rId4"/>
+    <sheet name="hb_node" sheetId="6" r:id="rId2"/>
+    <sheet name="kfk_node" sheetId="3" r:id="rId3"/>
+    <sheet name="msq_msq_rule" sheetId="4" r:id="rId4"/>
+    <sheet name="msq_kfk_rule" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="378">
   <si>
     <t>}</t>
   </si>
@@ -1166,6 +1167,12 @@
   </si>
   <si>
     <t>"pass"</t>
+  </si>
+  <si>
+    <t>8020</t>
+  </si>
+  <si>
+    <t>"hbase"</t>
   </si>
 </sst>
 </file>
@@ -1550,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC7696D2-C4F4-2248-BB46-E6E5934265D5}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1917,10 +1924,248 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DF4538-1A92-1940-92FF-2CF40E132735}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8AB31C-1058-4A4E-81E1-10A19260E2B0}">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
@@ -2799,7 +3044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF08169F-0E4C-E74B-9E8E-367D0426A774}">
   <dimension ref="A1:E191"/>
   <sheetViews>
@@ -4600,11 +4845,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3A68D5-58FD-DA42-BFF7-99C100BAE536}">
   <dimension ref="A1:E267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+    <sheetView topLeftCell="A237" workbookViewId="0">
       <selection activeCell="E265" sqref="E265"/>
     </sheetView>
   </sheetViews>

</xml_diff>